<commit_message>
Signed-off-by: Attila Koksal <akoksal@student.rccd.edu>
</commit_message>
<xml_diff>
--- a/Class/MidtermProblems/Question1/Question1.xlsx
+++ b/Class/MidtermProblems/Question1/Question1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attil\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e98a767685f68f6f/Desktop/CS17C/KoksalAttila_CIS17C_43484/Class/MidtermProblems/Question1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E1EB01E-C1C0-4111-8E0D-DB5880B44DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{5E1EB01E-C1C0-4111-8E0D-DB5880B44DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AC53AB2-C2C7-4888-A38F-6E32E090C478}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000E+00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +121,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -154,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -164,6 +173,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8045,7 +8055,7 @@
   <dimension ref="C4:AB42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8060,7 +8070,7 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
     </row>
@@ -8082,7 +8092,7 @@
       <c r="I6" s="1">
         <v>275.15800000000002</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="U6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="Z6" s="1" t="s">

</xml_diff>